<commit_message>
Wyświetlanie w DCV, poprawa błędów
</commit_message>
<xml_diff>
--- a/Zapis_Swiadectw_Wzorcowania/nazwa_pliku.xlsx
+++ b/Zapis_Swiadectw_Wzorcowania/nazwa_pliku.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>1</col>
@@ -193,13 +193,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -491,7 +491,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -543,7 +543,7 @@
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>06.03.2023</t>
+          <t>07.03.2023</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>06.03.2023</t>
+          <t>07.03.2023</t>
         </is>
       </c>
       <c r="D11" s="1" t="n"/>
@@ -742,6 +742,6 @@
     <mergeCell ref="C10:E10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pkt.P. + SW bez PktP.
</commit_message>
<xml_diff>
--- a/Zapis_Swiadectw_Wzorcowania/nazwa_pliku.xlsx
+++ b/Zapis_Swiadectw_Wzorcowania/nazwa_pliku.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="132" yWindow="516" windowWidth="22716" windowHeight="8940" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="32520" yWindow="2415" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Swiadectwo" sheetId="1" state="visible" r:id="rId1"/>
@@ -68,6 +68,30 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -173,30 +197,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="00000000"/>
       </left>
@@ -248,20 +248,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -828,13 +828,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="1" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="13.6640625" customWidth="1" min="3" max="3"/>
-    <col width="30.5546875" customWidth="1" min="4" max="4"/>
-    <col width="20.88671875" customWidth="1" min="5" max="5"/>
+    <col width="13.7109375" customWidth="1" min="3" max="3"/>
+    <col width="30.5703125" customWidth="1" min="4" max="4"/>
+    <col width="20.85546875" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="2" ht="90" customHeight="1">
@@ -848,8 +848,8 @@
 www.metro-lab.pl</t>
         </is>
       </c>
-      <c r="D2" s="16" t="n"/>
-      <c r="E2" s="17" t="n"/>
+      <c r="D2" s="13" t="n"/>
+      <c r="E2" s="14" t="n"/>
     </row>
     <row r="3" ht="41.25" customHeight="1">
       <c r="B3" s="9" t="inlineStr">
@@ -857,9 +857,9 @@
           <t>ŚWIADECTWO WZORCOWANIA</t>
         </is>
       </c>
-      <c r="C3" s="16" t="n"/>
-      <c r="D3" s="16" t="n"/>
-      <c r="E3" s="17" t="n"/>
+      <c r="C3" s="13" t="n"/>
+      <c r="D3" s="13" t="n"/>
+      <c r="E3" s="14" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="B4" s="8" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="C4" s="8" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="D4" s="8" t="inlineStr">
@@ -884,10 +884,10 @@
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="B5" s="15" t="n"/>
-      <c r="C5" s="15" t="n"/>
-      <c r="D5" s="15" t="n"/>
-      <c r="E5" s="15" t="n"/>
+      <c r="B5" s="17" t="n"/>
+      <c r="C5" s="17" t="n"/>
+      <c r="D5" s="17" t="n"/>
+      <c r="E5" s="17" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="B6" s="2" t="n"/>
@@ -905,8 +905,8 @@
           <t xml:space="preserve">Multimetr [MODEL], nr </t>
         </is>
       </c>
-      <c r="D7" s="16" t="n"/>
-      <c r="E7" s="17" t="n"/>
+      <c r="D7" s="13" t="n"/>
+      <c r="E7" s="14" t="n"/>
     </row>
     <row r="8" ht="45.75" customHeight="1">
       <c r="B8" s="11" t="inlineStr">
@@ -921,8 +921,8 @@
 00-034 Warszawa</t>
         </is>
       </c>
-      <c r="D8" s="16" t="n"/>
-      <c r="E8" s="17" t="n"/>
+      <c r="D8" s="13" t="n"/>
+      <c r="E8" s="14" t="n"/>
     </row>
     <row r="9" ht="37.5" customHeight="1">
       <c r="B9" s="11" t="inlineStr">
@@ -936,8 +936,8 @@
           <t>Procedura pomiarowa PW005 wydanie 2</t>
         </is>
       </c>
-      <c r="D9" s="16" t="n"/>
-      <c r="E9" s="17" t="n"/>
+      <c r="D9" s="13" t="n"/>
+      <c r="E9" s="14" t="n"/>
     </row>
     <row r="10" ht="48" customHeight="1">
       <c r="B10" s="11" t="inlineStr">
@@ -952,8 +952,8 @@
 Wilgotność   (42 ÷ 47) %</t>
         </is>
       </c>
-      <c r="D10" s="16" t="n"/>
-      <c r="E10" s="17" t="n"/>
+      <c r="D10" s="13" t="n"/>
+      <c r="E10" s="14" t="n"/>
     </row>
     <row r="11" ht="37.5" customHeight="1">
       <c r="B11" s="11" t="inlineStr">
@@ -964,11 +964,11 @@
       </c>
       <c r="C11" s="8" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
-        </is>
-      </c>
-      <c r="D11" s="16" t="n"/>
-      <c r="E11" s="17" t="n"/>
+          <t>15.04.2023</t>
+        </is>
+      </c>
+      <c r="D11" s="13" t="n"/>
+      <c r="E11" s="14" t="n"/>
     </row>
     <row r="12" ht="79.5" customHeight="1">
       <c r="B12" s="11" t="inlineStr">
@@ -982,8 +982,8 @@
           <t>Wyniki wzorcowania miernika zostały odniesione do wzorców państwowych przy wykorzystaniu multimetru wzorcowego: ...</t>
         </is>
       </c>
-      <c r="D12" s="16" t="n"/>
-      <c r="E12" s="17" t="n"/>
+      <c r="D12" s="13" t="n"/>
+      <c r="E12" s="14" t="n"/>
     </row>
     <row r="13" ht="108.75" customHeight="1">
       <c r="B13" s="11" t="inlineStr">
@@ -997,8 +997,8 @@
           <t>Niepewność pomiaru została określona zgodnie z dokumentem EA-4/02 M:2021. Podane wartości niepewności stanowią niepewności rozszerzone przy prawdopodobieństwie rozszerzenia ok. 95 % i współczynniku rozszerzenia k = 2</t>
         </is>
       </c>
-      <c r="D13" s="16" t="n"/>
-      <c r="E13" s="17" t="n"/>
+      <c r="D13" s="13" t="n"/>
+      <c r="E13" s="14" t="n"/>
     </row>
     <row r="14" ht="37.5" customHeight="1">
       <c r="B14" s="11" t="inlineStr">
@@ -1012,8 +1012,8 @@
           <t>Podano na kolejnych stronach niniejszego świadectwa</t>
         </is>
       </c>
-      <c r="D14" s="16" t="n"/>
-      <c r="E14" s="17" t="n"/>
+      <c r="D14" s="13" t="n"/>
+      <c r="E14" s="14" t="n"/>
     </row>
     <row r="15">
       <c r="B15" s="10" t="inlineStr">
@@ -1080,13 +1080,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -1097,6 +1097,7 @@
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="92" customHeight="1">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
@@ -1136,7 +1137,7 @@
       <c r="B4" s="25" t="n"/>
       <c r="C4" s="28" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="D4" s="28" t="inlineStr">
@@ -1152,6 +1153,8 @@
         </is>
       </c>
     </row>
+    <row r="5"/>
+    <row r="6"/>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
@@ -1180,6 +1183,7 @@
         </is>
       </c>
     </row>
+    <row r="11"/>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
@@ -1187,7 +1191,9 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="39.6" customHeight="1">
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15" ht="38.25" customHeight="1">
       <c r="B15" s="10" t="inlineStr">
         <is>
           <t>Zakres</t>
@@ -1215,216 +1221,198 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="13" t="inlineStr">
+      <c r="B16" s="15" t="inlineStr">
         <is>
           <t>mV</t>
         </is>
       </c>
-      <c r="C16" s="16" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
-      <c r="F16" s="17" t="n"/>
+      <c r="C16" s="13" t="n"/>
+      <c r="D16" s="13" t="n"/>
+      <c r="E16" s="14" t="n"/>
+      <c r="F16" s="15" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="13" t="n">
-        <v>400</v>
-      </c>
-      <c r="C17" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="D17" s="13" t="n"/>
-      <c r="E17" s="13" t="n"/>
-      <c r="F17" s="13" t="n"/>
+      <c r="B17" s="15" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D17" s="15" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="E17" s="15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F17" s="15" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="14" t="n"/>
-      <c r="C18" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="D18" s="13" t="n"/>
-      <c r="E18" s="13" t="n"/>
-      <c r="F18" s="13" t="n"/>
+      <c r="B18" s="16" t="n"/>
+      <c r="C18" s="15" t="n"/>
+      <c r="D18" s="15" t="n"/>
+      <c r="E18" s="15" t="n"/>
+      <c r="F18" s="15" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="14" t="n"/>
-      <c r="C19" s="13" t="n">
-        <v>360</v>
-      </c>
-      <c r="D19" s="13" t="n"/>
-      <c r="E19" s="13" t="n"/>
-      <c r="F19" s="13" t="n"/>
+      <c r="B19" s="16" t="n"/>
+      <c r="C19" s="15" t="n"/>
+      <c r="D19" s="15" t="n"/>
+      <c r="E19" s="15" t="n"/>
+      <c r="F19" s="15" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="15" t="n"/>
-      <c r="C20" s="13" t="n">
-        <v>-360</v>
-      </c>
-      <c r="D20" s="13" t="n"/>
-      <c r="E20" s="13" t="n"/>
-      <c r="F20" s="13" t="n"/>
+      <c r="B20" s="17" t="n"/>
+      <c r="C20" s="15" t="n"/>
+      <c r="D20" s="15" t="n"/>
+      <c r="E20" s="15" t="n"/>
+      <c r="F20" s="15" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="13" t="inlineStr">
+      <c r="B21" s="15" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="C21" s="16" t="n"/>
-      <c r="D21" s="16" t="n"/>
-      <c r="E21" s="16" t="n"/>
-      <c r="F21" s="17" t="n"/>
+      <c r="C21" s="13" t="n"/>
+      <c r="D21" s="13" t="n"/>
+      <c r="E21" s="14" t="n"/>
+      <c r="F21" s="15" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="C22" s="13" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D22" s="13" t="n"/>
-      <c r="E22" s="13" t="n"/>
-      <c r="F22" s="13" t="n"/>
+      <c r="B22" s="15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C22" s="15" t="n"/>
+      <c r="D22" s="15" t="n"/>
+      <c r="E22" s="15" t="n"/>
+      <c r="F22" s="15" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="14" t="n"/>
-      <c r="C23" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" s="13" t="n"/>
-      <c r="E23" s="13" t="n"/>
-      <c r="F23" s="13" t="n"/>
+      <c r="B23" s="16" t="n"/>
+      <c r="C23" s="15" t="n"/>
+      <c r="D23" s="15" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="14" t="n"/>
-      <c r="C24" s="13" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="D24" s="13" t="n"/>
-      <c r="E24" s="13" t="n"/>
-      <c r="F24" s="13" t="n"/>
+      <c r="B24" s="16" t="n"/>
+      <c r="C24" s="15" t="n"/>
+      <c r="D24" s="15" t="n"/>
+      <c r="E24" s="15" t="n"/>
+      <c r="F24" s="15" t="n"/>
     </row>
     <row r="25">
-      <c r="B25" s="15" t="n"/>
-      <c r="C25" s="13" t="n">
-        <v>-3.6</v>
-      </c>
-      <c r="D25" s="13" t="n"/>
-      <c r="E25" s="13" t="n"/>
-      <c r="F25" s="13" t="n"/>
+      <c r="B25" s="17" t="n"/>
+      <c r="C25" s="15" t="n"/>
+      <c r="D25" s="15" t="n"/>
+      <c r="E25" s="15" t="n"/>
+      <c r="F25" s="15" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="C26" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="D26" s="13" t="n"/>
-      <c r="E26" s="13" t="n"/>
-      <c r="F26" s="13" t="n"/>
+      <c r="B26" s="15" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C26" s="15" t="n"/>
+      <c r="D26" s="15" t="n"/>
+      <c r="E26" s="15" t="n"/>
+      <c r="F26" s="15" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" s="14" t="n"/>
-      <c r="C27" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D27" s="13" t="n"/>
-      <c r="E27" s="13" t="n"/>
-      <c r="F27" s="13" t="n"/>
+      <c r="B27" s="16" t="n"/>
+      <c r="C27" s="15" t="n"/>
+      <c r="D27" s="15" t="n"/>
+      <c r="E27" s="15" t="n"/>
+      <c r="F27" s="15" t="n"/>
     </row>
     <row r="28">
-      <c r="B28" s="14" t="n"/>
-      <c r="C28" s="13" t="n">
-        <v>36</v>
-      </c>
-      <c r="D28" s="13" t="n"/>
-      <c r="E28" s="13" t="n"/>
-      <c r="F28" s="13" t="n"/>
+      <c r="B28" s="16" t="n"/>
+      <c r="C28" s="15" t="n"/>
+      <c r="D28" s="15" t="n"/>
+      <c r="E28" s="15" t="n"/>
+      <c r="F28" s="15" t="n"/>
     </row>
     <row r="29">
-      <c r="B29" s="15" t="n"/>
-      <c r="C29" s="13" t="n">
-        <v>-36</v>
-      </c>
-      <c r="D29" s="13" t="n"/>
-      <c r="E29" s="13" t="n"/>
-      <c r="F29" s="13" t="n"/>
+      <c r="B29" s="17" t="n"/>
+      <c r="C29" s="15" t="n"/>
+      <c r="D29" s="15" t="n"/>
+      <c r="E29" s="15" t="n"/>
+      <c r="F29" s="15" t="n"/>
     </row>
     <row r="30">
-      <c r="B30" s="13" t="n">
-        <v>400</v>
-      </c>
-      <c r="C30" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="D30" s="13" t="n"/>
-      <c r="E30" s="13" t="n"/>
-      <c r="F30" s="13" t="n"/>
+      <c r="B30" s="15" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C30" s="15" t="n"/>
+      <c r="D30" s="15" t="n"/>
+      <c r="E30" s="15" t="n"/>
+      <c r="F30" s="15" t="n"/>
     </row>
     <row r="31">
-      <c r="B31" s="14" t="n"/>
-      <c r="C31" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="D31" s="13" t="n"/>
-      <c r="E31" s="13" t="n"/>
-      <c r="F31" s="13" t="n"/>
+      <c r="B31" s="16" t="n"/>
+      <c r="C31" s="15" t="n"/>
+      <c r="D31" s="15" t="n"/>
+      <c r="E31" s="15" t="n"/>
+      <c r="F31" s="15" t="n"/>
     </row>
     <row r="32">
-      <c r="B32" s="14" t="n"/>
-      <c r="C32" s="13" t="n">
-        <v>360</v>
-      </c>
-      <c r="D32" s="13" t="n"/>
-      <c r="E32" s="13" t="n"/>
-      <c r="F32" s="13" t="n"/>
+      <c r="B32" s="16" t="n"/>
+      <c r="C32" s="15" t="n"/>
+      <c r="D32" s="15" t="n"/>
+      <c r="E32" s="15" t="n"/>
+      <c r="F32" s="15" t="n"/>
     </row>
     <row r="33">
-      <c r="B33" s="15" t="n"/>
-      <c r="C33" s="13" t="n">
-        <v>-360</v>
-      </c>
-      <c r="D33" s="13" t="n"/>
-      <c r="E33" s="13" t="n"/>
-      <c r="F33" s="13" t="n"/>
+      <c r="B33" s="17" t="n"/>
+      <c r="C33" s="15" t="n"/>
+      <c r="D33" s="15" t="n"/>
+      <c r="E33" s="15" t="n"/>
+      <c r="F33" s="15" t="n"/>
     </row>
     <row r="34">
-      <c r="B34" s="13" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C34" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="D34" s="13" t="n"/>
-      <c r="E34" s="13" t="n"/>
-      <c r="F34" s="13" t="n"/>
+      <c r="B34" s="15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C34" s="15" t="n"/>
+      <c r="D34" s="15" t="n"/>
+      <c r="E34" s="15" t="n"/>
+      <c r="F34" s="15" t="n"/>
     </row>
     <row r="35">
-      <c r="B35" s="14" t="n"/>
-      <c r="C35" s="13" t="n">
-        <v>500</v>
-      </c>
-      <c r="D35" s="13" t="n"/>
-      <c r="E35" s="13" t="n"/>
-      <c r="F35" s="13" t="n"/>
+      <c r="B35" s="16" t="n"/>
+      <c r="C35" s="15" t="n"/>
+      <c r="D35" s="15" t="n"/>
+      <c r="E35" s="15" t="n"/>
+      <c r="F35" s="15" t="n"/>
     </row>
     <row r="36">
-      <c r="B36" s="14" t="n"/>
-      <c r="C36" s="13" t="n">
-        <v>900</v>
-      </c>
-      <c r="D36" s="13" t="n"/>
-      <c r="E36" s="13" t="n"/>
-      <c r="F36" s="13" t="n"/>
+      <c r="B36" s="16" t="n"/>
+      <c r="C36" s="15" t="n"/>
+      <c r="D36" s="15" t="n"/>
+      <c r="E36" s="15" t="n"/>
+      <c r="F36" s="15" t="n"/>
     </row>
     <row r="37">
-      <c r="B37" s="15" t="n"/>
-      <c r="C37" s="13" t="n">
-        <v>-900</v>
-      </c>
-      <c r="D37" s="13" t="n"/>
-      <c r="E37" s="13" t="n"/>
-      <c r="F37" s="13" t="n"/>
+      <c r="B37" s="17" t="n"/>
+      <c r="C37" s="15" t="n"/>
+      <c r="D37" s="15" t="n"/>
+      <c r="E37" s="15" t="n"/>
+      <c r="F37" s="15" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1460,13 +1448,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -1477,6 +1465,7 @@
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="92" customHeight="1">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
@@ -1516,7 +1505,7 @@
       <c r="B4" s="25" t="n"/>
       <c r="C4" s="28" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="D4" s="28" t="inlineStr">
@@ -1532,6 +1521,13 @@
         </is>
       </c>
     </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
@@ -1546,7 +1542,8 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="39.6" customHeight="1">
+    <row r="14"/>
+    <row r="15" ht="38.25" customHeight="1">
       <c r="B15" s="10" t="inlineStr">
         <is>
           <t>Zakres</t>
@@ -1574,91 +1571,79 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="13" t="inlineStr">
+      <c r="B16" s="15" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="C16" s="16" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
-      <c r="F16" s="17" t="n"/>
+      <c r="C16" s="13" t="n"/>
+      <c r="D16" s="13" t="n"/>
+      <c r="E16" s="14" t="n"/>
+      <c r="F16" s="15" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="13" t="n">
-        <v>400</v>
-      </c>
-      <c r="C17" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="D17" s="13" t="n"/>
-      <c r="E17" s="13" t="n"/>
-      <c r="F17" s="13" t="n"/>
+      <c r="B17" s="15" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C17" s="15" t="n"/>
+      <c r="D17" s="15" t="n"/>
+      <c r="E17" s="15" t="n"/>
+      <c r="F17" s="15" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="14" t="n"/>
-      <c r="C18" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="D18" s="13" t="n"/>
-      <c r="E18" s="13" t="n"/>
-      <c r="F18" s="13" t="n"/>
+      <c r="B18" s="16" t="n"/>
+      <c r="C18" s="15" t="n"/>
+      <c r="D18" s="15" t="n"/>
+      <c r="E18" s="15" t="n"/>
+      <c r="F18" s="15" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="14" t="n"/>
-      <c r="C19" s="13" t="n">
-        <v>360</v>
-      </c>
-      <c r="D19" s="13" t="n"/>
-      <c r="E19" s="13" t="n"/>
-      <c r="F19" s="13" t="n"/>
+      <c r="B19" s="16" t="n"/>
+      <c r="C19" s="15" t="n"/>
+      <c r="D19" s="15" t="n"/>
+      <c r="E19" s="15" t="n"/>
+      <c r="F19" s="15" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="15" t="n"/>
-      <c r="C20" s="13" t="n">
-        <v>-360</v>
-      </c>
-      <c r="D20" s="13" t="n"/>
-      <c r="E20" s="13" t="n"/>
-      <c r="F20" s="13" t="n"/>
+      <c r="B20" s="17" t="n"/>
+      <c r="C20" s="15" t="n"/>
+      <c r="D20" s="15" t="n"/>
+      <c r="E20" s="15" t="n"/>
+      <c r="F20" s="15" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="13" t="n">
-        <v>750</v>
-      </c>
-      <c r="C21" s="13" t="n">
-        <v>75</v>
-      </c>
-      <c r="D21" s="13" t="n"/>
-      <c r="E21" s="13" t="n"/>
-      <c r="F21" s="13" t="n"/>
+      <c r="B21" s="15" t="inlineStr">
+        <is>
+          <t>750</t>
+        </is>
+      </c>
+      <c r="C21" s="15" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="15" t="n"/>
+      <c r="F21" s="15" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="14" t="n"/>
-      <c r="C22" s="13" t="n">
-        <v>375</v>
-      </c>
-      <c r="D22" s="13" t="n"/>
-      <c r="E22" s="13" t="n"/>
-      <c r="F22" s="13" t="n"/>
+      <c r="B22" s="16" t="n"/>
+      <c r="C22" s="15" t="n"/>
+      <c r="D22" s="15" t="n"/>
+      <c r="E22" s="15" t="n"/>
+      <c r="F22" s="15" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="14" t="n"/>
-      <c r="C23" s="13" t="n">
-        <v>675</v>
-      </c>
-      <c r="D23" s="13" t="n"/>
-      <c r="E23" s="13" t="n"/>
-      <c r="F23" s="13" t="n"/>
+      <c r="B23" s="16" t="n"/>
+      <c r="C23" s="15" t="n"/>
+      <c r="D23" s="15" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="15" t="n"/>
-      <c r="C24" s="13" t="n">
-        <v>-675</v>
-      </c>
-      <c r="D24" s="13" t="n"/>
-      <c r="E24" s="13" t="n"/>
-      <c r="F24" s="13" t="n"/>
+      <c r="B24" s="17" t="n"/>
+      <c r="C24" s="15" t="n"/>
+      <c r="D24" s="15" t="n"/>
+      <c r="E24" s="15" t="n"/>
+      <c r="F24" s="15" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1690,13 +1675,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -1707,6 +1692,7 @@
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="92" customHeight="1">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
@@ -1746,7 +1732,7 @@
       <c r="B4" s="25" t="n"/>
       <c r="C4" s="28" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="D4" s="28" t="inlineStr">
@@ -1762,6 +1748,13 @@
         </is>
       </c>
     </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
@@ -1769,7 +1762,9 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="39.6" customHeight="1">
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15" ht="38.25" customHeight="1">
       <c r="B15" s="10" t="inlineStr">
         <is>
           <t>Zakres</t>
@@ -1797,178 +1792,154 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="13" t="inlineStr">
+      <c r="B16" s="15" t="inlineStr">
         <is>
           <t>mA</t>
         </is>
       </c>
-      <c r="C16" s="16" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
-      <c r="F16" s="17" t="n"/>
+      <c r="C16" s="13" t="n"/>
+      <c r="D16" s="13" t="n"/>
+      <c r="E16" s="14" t="n"/>
+      <c r="F16" s="15" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" s="13" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D17" s="13" t="n"/>
-      <c r="E17" s="13" t="n"/>
-      <c r="F17" s="13" t="n"/>
+      <c r="B17" s="15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C17" s="15" t="n"/>
+      <c r="D17" s="15" t="n"/>
+      <c r="E17" s="15" t="n"/>
+      <c r="F17" s="15" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="14" t="n"/>
-      <c r="C18" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" s="13" t="n"/>
-      <c r="E18" s="13" t="n"/>
-      <c r="F18" s="13" t="n"/>
+      <c r="B18" s="16" t="n"/>
+      <c r="C18" s="15" t="n"/>
+      <c r="D18" s="15" t="n"/>
+      <c r="E18" s="15" t="n"/>
+      <c r="F18" s="15" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="14" t="n"/>
-      <c r="C19" s="13" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="D19" s="13" t="n"/>
-      <c r="E19" s="13" t="n"/>
-      <c r="F19" s="13" t="n"/>
+      <c r="B19" s="16" t="n"/>
+      <c r="C19" s="15" t="n"/>
+      <c r="D19" s="15" t="n"/>
+      <c r="E19" s="15" t="n"/>
+      <c r="F19" s="15" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="15" t="n"/>
-      <c r="C20" s="13" t="n">
-        <v>-3.6</v>
-      </c>
-      <c r="D20" s="13" t="n"/>
-      <c r="E20" s="13" t="n"/>
-      <c r="F20" s="13" t="n"/>
+      <c r="B20" s="17" t="n"/>
+      <c r="C20" s="15" t="n"/>
+      <c r="D20" s="15" t="n"/>
+      <c r="E20" s="15" t="n"/>
+      <c r="F20" s="15" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="C21" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" s="13" t="n"/>
-      <c r="E21" s="13" t="n"/>
-      <c r="F21" s="13" t="n"/>
+      <c r="B21" s="15" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C21" s="15" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="15" t="n"/>
+      <c r="F21" s="15" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="14" t="n"/>
-      <c r="C22" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D22" s="13" t="n"/>
-      <c r="E22" s="13" t="n"/>
-      <c r="F22" s="13" t="n"/>
+      <c r="B22" s="16" t="n"/>
+      <c r="C22" s="15" t="n"/>
+      <c r="D22" s="15" t="n"/>
+      <c r="E22" s="15" t="n"/>
+      <c r="F22" s="15" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="14" t="n"/>
-      <c r="C23" s="13" t="n">
-        <v>36</v>
-      </c>
-      <c r="D23" s="13" t="n"/>
-      <c r="E23" s="13" t="n"/>
-      <c r="F23" s="13" t="n"/>
+      <c r="B23" s="16" t="n"/>
+      <c r="C23" s="15" t="n"/>
+      <c r="D23" s="15" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="15" t="n"/>
-      <c r="C24" s="13" t="n">
-        <v>-36</v>
-      </c>
-      <c r="D24" s="13" t="n"/>
-      <c r="E24" s="13" t="n"/>
-      <c r="F24" s="13" t="n"/>
+      <c r="B24" s="17" t="n"/>
+      <c r="C24" s="15" t="n"/>
+      <c r="D24" s="15" t="n"/>
+      <c r="E24" s="15" t="n"/>
+      <c r="F24" s="15" t="n"/>
     </row>
     <row r="25">
-      <c r="B25" s="13" t="n">
-        <v>400</v>
-      </c>
-      <c r="C25" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="D25" s="13" t="n"/>
-      <c r="E25" s="13" t="n"/>
-      <c r="F25" s="13" t="n"/>
+      <c r="B25" s="15" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C25" s="15" t="n"/>
+      <c r="D25" s="15" t="n"/>
+      <c r="E25" s="15" t="n"/>
+      <c r="F25" s="15" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="14" t="n"/>
-      <c r="C26" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="D26" s="13" t="n"/>
-      <c r="E26" s="13" t="n"/>
-      <c r="F26" s="13" t="n"/>
+      <c r="B26" s="16" t="n"/>
+      <c r="C26" s="15" t="n"/>
+      <c r="D26" s="15" t="n"/>
+      <c r="E26" s="15" t="n"/>
+      <c r="F26" s="15" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" s="14" t="n"/>
-      <c r="C27" s="13" t="n">
-        <v>360</v>
-      </c>
-      <c r="D27" s="13" t="n"/>
-      <c r="E27" s="13" t="n"/>
-      <c r="F27" s="13" t="n"/>
+      <c r="B27" s="16" t="n"/>
+      <c r="C27" s="15" t="n"/>
+      <c r="D27" s="15" t="n"/>
+      <c r="E27" s="15" t="n"/>
+      <c r="F27" s="15" t="n"/>
     </row>
     <row r="28">
-      <c r="B28" s="15" t="n"/>
-      <c r="C28" s="13" t="n">
-        <v>-360</v>
-      </c>
-      <c r="D28" s="13" t="n"/>
-      <c r="E28" s="13" t="n"/>
-      <c r="F28" s="13" t="n"/>
+      <c r="B28" s="17" t="n"/>
+      <c r="C28" s="15" t="n"/>
+      <c r="D28" s="15" t="n"/>
+      <c r="E28" s="15" t="n"/>
+      <c r="F28" s="15" t="n"/>
     </row>
     <row r="29">
-      <c r="B29" s="13" t="inlineStr">
+      <c r="B29" s="15" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C29" s="16" t="n"/>
-      <c r="D29" s="16" t="n"/>
-      <c r="E29" s="16" t="n"/>
-      <c r="F29" s="17" t="n"/>
+      <c r="C29" s="13" t="n"/>
+      <c r="D29" s="13" t="n"/>
+      <c r="E29" s="14" t="n"/>
+      <c r="F29" s="15" t="n"/>
     </row>
     <row r="30">
-      <c r="B30" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="C30" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="13" t="n"/>
-      <c r="E30" s="13" t="n"/>
-      <c r="F30" s="13" t="n"/>
+      <c r="B30" s="15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C30" s="15" t="n"/>
+      <c r="D30" s="15" t="n"/>
+      <c r="E30" s="15" t="n"/>
+      <c r="F30" s="15" t="n"/>
     </row>
     <row r="31">
-      <c r="B31" s="14" t="n"/>
-      <c r="C31" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="D31" s="13" t="n"/>
-      <c r="E31" s="13" t="n"/>
-      <c r="F31" s="13" t="n"/>
+      <c r="B31" s="16" t="n"/>
+      <c r="C31" s="15" t="n"/>
+      <c r="D31" s="15" t="n"/>
+      <c r="E31" s="15" t="n"/>
+      <c r="F31" s="15" t="n"/>
     </row>
     <row r="32">
-      <c r="B32" s="14" t="n"/>
-      <c r="C32" s="13" t="n">
-        <v>9</v>
-      </c>
-      <c r="D32" s="13" t="n"/>
-      <c r="E32" s="13" t="n"/>
-      <c r="F32" s="13" t="n"/>
+      <c r="B32" s="16" t="n"/>
+      <c r="C32" s="15" t="n"/>
+      <c r="D32" s="15" t="n"/>
+      <c r="E32" s="15" t="n"/>
+      <c r="F32" s="15" t="n"/>
     </row>
     <row r="33">
-      <c r="B33" s="15" t="n"/>
-      <c r="C33" s="13" t="n">
-        <v>-9</v>
-      </c>
-      <c r="D33" s="13" t="n"/>
-      <c r="E33" s="13" t="n"/>
-      <c r="F33" s="13" t="n"/>
+      <c r="B33" s="17" t="n"/>
+      <c r="C33" s="15" t="n"/>
+      <c r="D33" s="15" t="n"/>
+      <c r="E33" s="15" t="n"/>
+      <c r="F33" s="15" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2003,13 +1974,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -2020,6 +1991,7 @@
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="92" customHeight="1">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
@@ -2059,7 +2031,7 @@
       <c r="B4" s="25" t="n"/>
       <c r="C4" s="28" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="D4" s="28" t="inlineStr">
@@ -2075,6 +2047,13 @@
         </is>
       </c>
     </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
@@ -2089,7 +2068,8 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="39.6" customHeight="1">
+    <row r="14"/>
+    <row r="15" ht="38.25" customHeight="1">
       <c r="B15" s="10" t="inlineStr">
         <is>
           <t>Zakres</t>
@@ -2117,140 +2097,122 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="13" t="inlineStr">
+      <c r="B16" s="15" t="inlineStr">
         <is>
           <t>mA</t>
         </is>
       </c>
-      <c r="C16" s="16" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
-      <c r="F16" s="17" t="n"/>
+      <c r="C16" s="13" t="n"/>
+      <c r="D16" s="13" t="n"/>
+      <c r="E16" s="14" t="n"/>
+      <c r="F16" s="15" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="C17" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="D17" s="13" t="n"/>
-      <c r="E17" s="13" t="n"/>
-      <c r="F17" s="13" t="n"/>
+      <c r="B17" s="15" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C17" s="15" t="n"/>
+      <c r="D17" s="15" t="n"/>
+      <c r="E17" s="15" t="n"/>
+      <c r="F17" s="15" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="14" t="n"/>
-      <c r="C18" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D18" s="13" t="n"/>
-      <c r="E18" s="13" t="n"/>
-      <c r="F18" s="13" t="n"/>
+      <c r="B18" s="16" t="n"/>
+      <c r="C18" s="15" t="n"/>
+      <c r="D18" s="15" t="n"/>
+      <c r="E18" s="15" t="n"/>
+      <c r="F18" s="15" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="14" t="n"/>
-      <c r="C19" s="13" t="n">
-        <v>36</v>
-      </c>
-      <c r="D19" s="13" t="n"/>
-      <c r="E19" s="13" t="n"/>
-      <c r="F19" s="13" t="n"/>
+      <c r="B19" s="16" t="n"/>
+      <c r="C19" s="15" t="n"/>
+      <c r="D19" s="15" t="n"/>
+      <c r="E19" s="15" t="n"/>
+      <c r="F19" s="15" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="15" t="n"/>
-      <c r="C20" s="13" t="n">
-        <v>-36</v>
-      </c>
-      <c r="D20" s="13" t="n"/>
-      <c r="E20" s="13" t="n"/>
-      <c r="F20" s="13" t="n"/>
+      <c r="B20" s="17" t="n"/>
+      <c r="C20" s="15" t="n"/>
+      <c r="D20" s="15" t="n"/>
+      <c r="E20" s="15" t="n"/>
+      <c r="F20" s="15" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="13" t="n">
-        <v>400</v>
-      </c>
-      <c r="C21" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="D21" s="13" t="n"/>
-      <c r="E21" s="13" t="n"/>
-      <c r="F21" s="13" t="n"/>
+      <c r="B21" s="15" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="C21" s="15" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="15" t="n"/>
+      <c r="F21" s="15" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="14" t="n"/>
-      <c r="C22" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="D22" s="13" t="n"/>
-      <c r="E22" s="13" t="n"/>
-      <c r="F22" s="13" t="n"/>
+      <c r="B22" s="16" t="n"/>
+      <c r="C22" s="15" t="n"/>
+      <c r="D22" s="15" t="n"/>
+      <c r="E22" s="15" t="n"/>
+      <c r="F22" s="15" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="14" t="n"/>
-      <c r="C23" s="13" t="n">
-        <v>360</v>
-      </c>
-      <c r="D23" s="13" t="n"/>
-      <c r="E23" s="13" t="n"/>
-      <c r="F23" s="13" t="n"/>
+      <c r="B23" s="16" t="n"/>
+      <c r="C23" s="15" t="n"/>
+      <c r="D23" s="15" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="15" t="n"/>
-      <c r="C24" s="13" t="n">
-        <v>-360</v>
-      </c>
-      <c r="D24" s="13" t="n"/>
-      <c r="E24" s="13" t="n"/>
-      <c r="F24" s="13" t="n"/>
+      <c r="B24" s="17" t="n"/>
+      <c r="C24" s="15" t="n"/>
+      <c r="D24" s="15" t="n"/>
+      <c r="E24" s="15" t="n"/>
+      <c r="F24" s="15" t="n"/>
     </row>
     <row r="25">
-      <c r="B25" s="13" t="inlineStr">
+      <c r="B25" s="15" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C25" s="16" t="n"/>
-      <c r="D25" s="16" t="n"/>
-      <c r="E25" s="16" t="n"/>
-      <c r="F25" s="17" t="n"/>
+      <c r="C25" s="13" t="n"/>
+      <c r="D25" s="13" t="n"/>
+      <c r="E25" s="14" t="n"/>
+      <c r="F25" s="15" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="C26" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="13" t="n"/>
-      <c r="E26" s="13" t="n"/>
-      <c r="F26" s="13" t="n"/>
+      <c r="B26" s="15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C26" s="15" t="n"/>
+      <c r="D26" s="15" t="n"/>
+      <c r="E26" s="15" t="n"/>
+      <c r="F26" s="15" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" s="14" t="n"/>
-      <c r="C27" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="D27" s="13" t="n"/>
-      <c r="E27" s="13" t="n"/>
-      <c r="F27" s="13" t="n"/>
+      <c r="B27" s="16" t="n"/>
+      <c r="C27" s="15" t="n"/>
+      <c r="D27" s="15" t="n"/>
+      <c r="E27" s="15" t="n"/>
+      <c r="F27" s="15" t="n"/>
     </row>
     <row r="28">
-      <c r="B28" s="14" t="n"/>
-      <c r="C28" s="13" t="n">
-        <v>9</v>
-      </c>
-      <c r="D28" s="13" t="n"/>
-      <c r="E28" s="13" t="n"/>
-      <c r="F28" s="13" t="n"/>
+      <c r="B28" s="16" t="n"/>
+      <c r="C28" s="15" t="n"/>
+      <c r="D28" s="15" t="n"/>
+      <c r="E28" s="15" t="n"/>
+      <c r="F28" s="15" t="n"/>
     </row>
     <row r="29">
-      <c r="B29" s="15" t="n"/>
-      <c r="C29" s="13" t="n">
-        <v>-9</v>
-      </c>
-      <c r="D29" s="13" t="n"/>
-      <c r="E29" s="13" t="n"/>
-      <c r="F29" s="13" t="n"/>
+      <c r="B29" s="17" t="n"/>
+      <c r="C29" s="15" t="n"/>
+      <c r="D29" s="15" t="n"/>
+      <c r="E29" s="15" t="n"/>
+      <c r="F29" s="15" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2284,13 +2246,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -2301,6 +2263,7 @@
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2" ht="92" customHeight="1">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
@@ -2340,7 +2303,7 @@
       <c r="B4" s="25" t="n"/>
       <c r="C4" s="28" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="D4" s="28" t="inlineStr">
@@ -2356,6 +2319,13 @@
         </is>
       </c>
     </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
@@ -2363,7 +2333,9 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="39.6" customHeight="1">
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15" ht="38.25" customHeight="1">
       <c r="B15" s="10" t="inlineStr">
         <is>
           <t>Zakres</t>
@@ -2391,157 +2363,145 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="13" t="inlineStr">
+      <c r="B16" s="15" t="inlineStr">
         <is>
           <t>Ω</t>
         </is>
       </c>
-      <c r="C16" s="16" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
-      <c r="F16" s="17" t="n"/>
+      <c r="C16" s="13" t="n"/>
+      <c r="D16" s="13" t="n"/>
+      <c r="E16" s="14" t="n"/>
+      <c r="F16" s="15" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="C17" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D17" s="13" t="n"/>
-      <c r="E17" s="13" t="n"/>
-      <c r="F17" s="13" t="n"/>
+      <c r="B17" s="15" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="C17" s="15" t="n"/>
+      <c r="D17" s="15" t="n"/>
+      <c r="E17" s="15" t="n"/>
+      <c r="F17" s="15" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="15" t="n"/>
-      <c r="C18" s="13" t="n">
-        <v>180</v>
-      </c>
-      <c r="D18" s="13" t="n"/>
-      <c r="E18" s="13" t="n"/>
-      <c r="F18" s="13" t="n"/>
+      <c r="B18" s="17" t="n"/>
+      <c r="C18" s="15" t="n"/>
+      <c r="D18" s="15" t="n"/>
+      <c r="E18" s="15" t="n"/>
+      <c r="F18" s="15" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="13" t="inlineStr">
+      <c r="B19" s="15" t="inlineStr">
         <is>
           <t>kΩ</t>
         </is>
       </c>
-      <c r="C19" s="16" t="n"/>
-      <c r="D19" s="16" t="n"/>
-      <c r="E19" s="16" t="n"/>
-      <c r="F19" s="17" t="n"/>
+      <c r="C19" s="13" t="n"/>
+      <c r="D19" s="13" t="n"/>
+      <c r="E19" s="14" t="n"/>
+      <c r="F19" s="15" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" s="13" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D20" s="13" t="n"/>
-      <c r="E20" s="13" t="n"/>
-      <c r="F20" s="13" t="n"/>
+      <c r="B20" s="15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C20" s="15" t="n"/>
+      <c r="D20" s="15" t="n"/>
+      <c r="E20" s="15" t="n"/>
+      <c r="F20" s="15" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="15" t="n"/>
-      <c r="C21" s="13" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="D21" s="13" t="n"/>
-      <c r="E21" s="13" t="n"/>
-      <c r="F21" s="13" t="n"/>
+      <c r="B21" s="17" t="n"/>
+      <c r="C21" s="15" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="15" t="n"/>
+      <c r="F21" s="15" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="C22" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D22" s="13" t="n"/>
-      <c r="E22" s="13" t="n"/>
-      <c r="F22" s="13" t="n"/>
+      <c r="B22" s="15" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C22" s="15" t="n"/>
+      <c r="D22" s="15" t="n"/>
+      <c r="E22" s="15" t="n"/>
+      <c r="F22" s="15" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="15" t="n"/>
-      <c r="C23" s="13" t="n">
-        <v>18</v>
-      </c>
-      <c r="D23" s="13" t="n"/>
-      <c r="E23" s="13" t="n"/>
-      <c r="F23" s="13" t="n"/>
+      <c r="B23" s="17" t="n"/>
+      <c r="C23" s="15" t="n"/>
+      <c r="D23" s="15" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="C24" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D24" s="13" t="n"/>
-      <c r="E24" s="13" t="n"/>
-      <c r="F24" s="13" t="n"/>
+      <c r="B24" s="15" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="C24" s="15" t="n"/>
+      <c r="D24" s="15" t="n"/>
+      <c r="E24" s="15" t="n"/>
+      <c r="F24" s="15" t="n"/>
     </row>
     <row r="25">
-      <c r="B25" s="15" t="n"/>
-      <c r="C25" s="13" t="n">
-        <v>180</v>
-      </c>
-      <c r="D25" s="13" t="n"/>
-      <c r="E25" s="13" t="n"/>
-      <c r="F25" s="13" t="n"/>
+      <c r="B25" s="17" t="n"/>
+      <c r="C25" s="15" t="n"/>
+      <c r="D25" s="15" t="n"/>
+      <c r="E25" s="15" t="n"/>
+      <c r="F25" s="15" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="13" t="inlineStr">
+      <c r="B26" s="15" t="inlineStr">
         <is>
           <t>MΩ</t>
         </is>
       </c>
-      <c r="C26" s="16" t="n"/>
-      <c r="D26" s="16" t="n"/>
-      <c r="E26" s="16" t="n"/>
-      <c r="F26" s="17" t="n"/>
+      <c r="C26" s="13" t="n"/>
+      <c r="D26" s="13" t="n"/>
+      <c r="E26" s="14" t="n"/>
+      <c r="F26" s="15" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="C27" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="D27" s="13" t="n"/>
-      <c r="E27" s="13" t="n"/>
-      <c r="F27" s="13" t="n"/>
+      <c r="B27" s="15" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C27" s="15" t="n"/>
+      <c r="D27" s="15" t="n"/>
+      <c r="E27" s="15" t="n"/>
+      <c r="F27" s="15" t="n"/>
     </row>
     <row r="28">
-      <c r="B28" s="15" t="n"/>
-      <c r="C28" s="13" t="n">
-        <v>18</v>
-      </c>
-      <c r="D28" s="13" t="n"/>
-      <c r="E28" s="13" t="n"/>
-      <c r="F28" s="13" t="n"/>
+      <c r="B28" s="17" t="n"/>
+      <c r="C28" s="15" t="n"/>
+      <c r="D28" s="15" t="n"/>
+      <c r="E28" s="15" t="n"/>
+      <c r="F28" s="15" t="n"/>
     </row>
     <row r="29">
-      <c r="B29" s="13" t="n">
-        <v>200</v>
-      </c>
-      <c r="C29" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D29" s="13" t="n"/>
-      <c r="E29" s="13" t="n"/>
-      <c r="F29" s="13" t="n"/>
+      <c r="B29" s="15" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="C29" s="15" t="n"/>
+      <c r="D29" s="15" t="n"/>
+      <c r="E29" s="15" t="n"/>
+      <c r="F29" s="15" t="n"/>
     </row>
     <row r="30">
-      <c r="B30" s="15" t="n"/>
-      <c r="C30" s="13" t="n">
-        <v>180</v>
-      </c>
-      <c r="D30" s="13" t="n"/>
-      <c r="E30" s="13" t="n"/>
-      <c r="F30" s="13" t="n"/>
+      <c r="B30" s="17" t="n"/>
+      <c r="C30" s="15" t="n"/>
+      <c r="D30" s="15" t="n"/>
+      <c r="E30" s="15" t="n"/>
+      <c r="F30" s="15" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2585,7 +2545,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>